<commit_message>
added sensorposition relating cubesat powerbudget without angular rate 360deg
</commit_message>
<xml_diff>
--- a/ScanSat_Template_TB-Power_v0.1.xlsx
+++ b/ScanSat_Template_TB-Power_v0.1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Change-log" sheetId="1" state="visible" r:id="rId2"/>
@@ -1972,6 +1972,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1994,6 +1995,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -2001,6 +2003,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
@@ -2008,6 +2011,7 @@
       <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -2015,18 +2019,21 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -2035,6 +2042,7 @@
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -2042,6 +2050,7 @@
       <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -2049,6 +2058,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="9">
@@ -2492,7 +2502,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="135">
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2965,10 +2975,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3017,7 +3023,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3035,6 +3057,7 @@
     <dxf>
       <font>
         <name val="Calibri"/>
+        <charset val="1"/>
         <family val="2"/>
         <b val="0"/>
         <i val="0"/>
@@ -3047,18 +3070,17 @@
       <numFmt numFmtId="164" formatCode="0%"/>
       <fill>
         <patternFill>
-          <bgColor rgb="00FFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
     <dxf>
       <font>
         <name val="Calibri"/>
+        <charset val="1"/>
         <family val="2"/>
         <color rgb="FF000000"/>
       </font>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </dxf>
   </dxfs>
   <colors>
@@ -3138,9 +3160,9 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5708502024291"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="47.9878542510121"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="48.417004048583"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.6720647773279"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="23.8866396761134"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.5708502024291"/>
   </cols>
   <sheetData>
@@ -3437,23 +3459,23 @@
   </sheetPr>
   <dimension ref="C2:H8"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F19" activeCellId="0" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C2" s="118" t="s">
+      <c r="C2" s="115" t="s">
         <v>288</v>
       </c>
-      <c r="D2" s="118"/>
-      <c r="E2" s="118"/>
-      <c r="F2" s="118"/>
-      <c r="G2" s="118"/>
+      <c r="D2" s="115"/>
+      <c r="E2" s="115"/>
+      <c r="F2" s="115"/>
+      <c r="G2" s="115"/>
     </row>
     <row r="3" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C3" s="116" t="s">
@@ -4026,7 +4048,7 @@
   <dimension ref="A2:S19"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H24" activeCellId="0" sqref="H24"/>
+      <selection pane="topLeft" activeCell="N24" activeCellId="0" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4598,7 +4620,7 @@
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="4" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.9959514170041"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="15.1052631578947"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9.10526315789474"/>
   </cols>
@@ -4662,7 +4684,7 @@
       <c r="G5" s="0" t="n">
         <v>1.5</v>
       </c>
-      <c r="H5" s="119" t="s">
+      <c r="H5" s="118" t="s">
         <v>430</v>
       </c>
       <c r="I5" s="0" t="s">
@@ -4903,10 +4925,10 @@
       <c r="D16" s="117" t="s">
         <v>466</v>
       </c>
-      <c r="E16" s="120" t="n">
+      <c r="E16" s="119" t="n">
         <v>0.175</v>
       </c>
-      <c r="F16" s="120" t="n">
+      <c r="F16" s="119" t="n">
         <v>60</v>
       </c>
       <c r="G16" s="0" t="n">
@@ -4953,12 +4975,12 @@
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.5708502024291"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.6032388663968"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.3157894736842"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="21.5303643724696"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="0" width="10.9271255060729"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="10.8178137651822"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.8906882591093"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="14.9959514170041"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -5411,7 +5433,7 @@
       <c r="C24" s="117" t="s">
         <v>518</v>
       </c>
-      <c r="D24" s="120" t="n">
+      <c r="D24" s="119" t="n">
         <v>2</v>
       </c>
       <c r="E24" s="0" t="n">
@@ -5420,7 +5442,7 @@
       <c r="F24" s="117" t="n">
         <v>0.45</v>
       </c>
-      <c r="G24" s="120" t="n">
+      <c r="G24" s="119" t="n">
         <v>0.23</v>
       </c>
       <c r="H24" s="0" t="s">
@@ -5509,7 +5531,7 @@
   </sheetPr>
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
     </sheetView>
   </sheetViews>
@@ -5517,12 +5539,12 @@
   <cols>
     <col collapsed="false" hidden="false" max="2" min="1" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.0323886639676"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.1376518218623"/>
     <col collapsed="false" hidden="false" max="8" min="5" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="13.3886639676113"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="88.9068825910931"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="28.2793522267206"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.1376518218623"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="89.6599190283401"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="28.4939271255061"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="29.3522267206478"/>
     <col collapsed="false" hidden="false" max="1025" min="13" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -5536,17 +5558,17 @@
       <c r="H3" s="30"/>
     </row>
     <row r="4" customFormat="false" ht="20.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="C4" s="121" t="s">
+      <c r="C4" s="120" t="s">
         <v>524</v>
       </c>
-      <c r="D4" s="121"/>
-      <c r="E4" s="121"/>
-      <c r="F4" s="121"/>
-      <c r="G4" s="121"/>
-      <c r="H4" s="121" t="s">
+      <c r="D4" s="120"/>
+      <c r="E4" s="120"/>
+      <c r="F4" s="120"/>
+      <c r="G4" s="120"/>
+      <c r="H4" s="120" t="s">
         <v>525</v>
       </c>
-      <c r="I4" s="121"/>
+      <c r="I4" s="120"/>
     </row>
     <row r="5" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="116" t="s">
@@ -5576,25 +5598,25 @@
       <c r="A6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="122" t="s">
+      <c r="C6" s="121" t="s">
         <v>530</v>
       </c>
-      <c r="D6" s="122" t="s">
+      <c r="D6" s="121" t="s">
         <v>164</v>
       </c>
-      <c r="E6" s="122" t="n">
+      <c r="E6" s="121" t="n">
         <v>185</v>
       </c>
-      <c r="F6" s="122" t="s">
+      <c r="F6" s="121" t="s">
         <v>154</v>
       </c>
-      <c r="G6" s="122" t="n">
+      <c r="G6" s="121" t="n">
         <v>0.04</v>
       </c>
-      <c r="H6" s="123" t="s">
+      <c r="H6" s="122" t="s">
         <v>531</v>
       </c>
-      <c r="I6" s="123" t="s">
+      <c r="I6" s="122" t="s">
         <v>532</v>
       </c>
       <c r="J6" s="0" t="s">
@@ -5606,25 +5628,25 @@
       <c r="A7" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C7" s="122" t="s">
+      <c r="C7" s="121" t="s">
         <v>534</v>
       </c>
-      <c r="D7" s="122" t="s">
+      <c r="D7" s="121" t="s">
         <v>164</v>
       </c>
-      <c r="E7" s="122" t="s">
+      <c r="E7" s="121" t="s">
         <v>535</v>
       </c>
-      <c r="F7" s="122" t="n">
+      <c r="F7" s="121" t="n">
         <v>1</v>
       </c>
-      <c r="G7" s="122" t="n">
+      <c r="G7" s="121" t="n">
         <v>0.005</v>
       </c>
-      <c r="H7" s="123" t="s">
+      <c r="H7" s="122" t="s">
         <v>536</v>
       </c>
-      <c r="I7" s="123" t="s">
+      <c r="I7" s="122" t="s">
         <v>537</v>
       </c>
       <c r="J7" s="0" t="s">
@@ -5636,25 +5658,25 @@
       <c r="A8" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C8" s="122" t="s">
+      <c r="C8" s="121" t="s">
         <v>538</v>
       </c>
-      <c r="D8" s="122" t="s">
+      <c r="D8" s="121" t="s">
         <v>164</v>
       </c>
-      <c r="E8" s="122" t="s">
+      <c r="E8" s="121" t="s">
         <v>539</v>
       </c>
-      <c r="F8" s="122" t="n">
+      <c r="F8" s="121" t="n">
         <v>1</v>
       </c>
-      <c r="G8" s="122" t="n">
+      <c r="G8" s="121" t="n">
         <v>0.018</v>
       </c>
-      <c r="H8" s="123" t="n">
+      <c r="H8" s="122" t="n">
         <v>1</v>
       </c>
-      <c r="I8" s="123" t="s">
+      <c r="I8" s="122" t="s">
         <v>540</v>
       </c>
       <c r="J8" s="0" t="s">
@@ -5666,25 +5688,25 @@
       <c r="A9" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C9" s="122" t="s">
+      <c r="C9" s="121" t="s">
         <v>541</v>
       </c>
-      <c r="D9" s="122" t="s">
+      <c r="D9" s="121" t="s">
         <v>164</v>
       </c>
-      <c r="E9" s="122" t="n">
+      <c r="E9" s="121" t="n">
         <v>226</v>
       </c>
-      <c r="F9" s="122" t="n">
+      <c r="F9" s="121" t="n">
         <v>20</v>
       </c>
-      <c r="G9" s="122" t="n">
+      <c r="G9" s="121" t="n">
         <v>0.18</v>
       </c>
-      <c r="H9" s="123" t="s">
+      <c r="H9" s="122" t="s">
         <v>542</v>
       </c>
-      <c r="I9" s="123" t="s">
+      <c r="I9" s="122" t="s">
         <v>543</v>
       </c>
       <c r="J9" s="0" t="s">
@@ -5695,25 +5717,25 @@
       <c r="A10" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C10" s="122" t="s">
+      <c r="C10" s="121" t="s">
         <v>544</v>
       </c>
-      <c r="D10" s="122" t="s">
+      <c r="D10" s="121" t="s">
         <v>545</v>
       </c>
-      <c r="E10" s="122" t="s">
+      <c r="E10" s="121" t="s">
         <v>546</v>
       </c>
-      <c r="F10" s="122" t="n">
+      <c r="F10" s="121" t="n">
         <v>4</v>
       </c>
-      <c r="G10" s="122" t="n">
+      <c r="G10" s="121" t="n">
         <v>0.015</v>
       </c>
-      <c r="H10" s="123" t="n">
+      <c r="H10" s="122" t="n">
         <v>1</v>
       </c>
-      <c r="I10" s="123" t="s">
+      <c r="I10" s="122" t="s">
         <v>547</v>
       </c>
       <c r="J10" s="0" t="s">
@@ -5724,25 +5746,25 @@
       <c r="A11" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="C11" s="122" t="s">
+      <c r="C11" s="121" t="s">
         <v>549</v>
       </c>
-      <c r="D11" s="122" t="s">
+      <c r="D11" s="121" t="s">
         <v>545</v>
       </c>
-      <c r="E11" s="122" t="s">
+      <c r="E11" s="121" t="s">
         <v>550</v>
       </c>
-      <c r="F11" s="122" t="n">
+      <c r="F11" s="121" t="n">
         <v>7</v>
       </c>
-      <c r="G11" s="122" t="n">
+      <c r="G11" s="121" t="n">
         <v>0.05</v>
       </c>
-      <c r="H11" s="123" t="n">
+      <c r="H11" s="122" t="n">
         <v>1</v>
       </c>
-      <c r="I11" s="123" t="s">
+      <c r="I11" s="122" t="s">
         <v>551</v>
       </c>
       <c r="J11" s="0" t="s">
@@ -5753,25 +5775,25 @@
       <c r="A12" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="C12" s="123" t="s">
+      <c r="C12" s="122" t="s">
         <v>552</v>
       </c>
-      <c r="D12" s="123" t="s">
+      <c r="D12" s="122" t="s">
         <v>444</v>
       </c>
-      <c r="E12" s="123" t="s">
+      <c r="E12" s="122" t="s">
         <v>553</v>
       </c>
-      <c r="F12" s="123" t="n">
+      <c r="F12" s="122" t="n">
         <v>12</v>
       </c>
-      <c r="G12" s="123" t="n">
+      <c r="G12" s="122" t="n">
         <v>0.05</v>
       </c>
-      <c r="H12" s="123" t="s">
+      <c r="H12" s="122" t="s">
         <v>554</v>
       </c>
-      <c r="I12" s="123" t="s">
+      <c r="I12" s="122" t="s">
         <v>555</v>
       </c>
       <c r="J12" s="0" t="s">
@@ -5782,25 +5804,25 @@
       <c r="A13" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="C13" s="123" t="s">
+      <c r="C13" s="122" t="s">
         <v>557</v>
       </c>
-      <c r="D13" s="123" t="s">
+      <c r="D13" s="122" t="s">
         <v>444</v>
       </c>
-      <c r="E13" s="123" t="s">
+      <c r="E13" s="122" t="s">
         <v>558</v>
       </c>
-      <c r="F13" s="123" t="s">
+      <c r="F13" s="122" t="s">
         <v>142</v>
       </c>
-      <c r="G13" s="123" t="n">
+      <c r="G13" s="122" t="n">
         <v>0.006</v>
       </c>
-      <c r="H13" s="123" t="n">
+      <c r="H13" s="122" t="n">
         <v>0.8</v>
       </c>
-      <c r="I13" s="123" t="s">
+      <c r="I13" s="122" t="s">
         <v>559</v>
       </c>
       <c r="J13" s="0" t="s">
@@ -5811,25 +5833,25 @@
       <c r="A14" s="0" t="n">
         <v>9</v>
       </c>
-      <c r="C14" s="123" t="s">
+      <c r="C14" s="122" t="s">
         <v>561</v>
       </c>
-      <c r="D14" s="123" t="s">
+      <c r="D14" s="122" t="s">
         <v>562</v>
       </c>
-      <c r="E14" s="123" t="n">
+      <c r="E14" s="122" t="n">
         <v>0.024</v>
       </c>
-      <c r="F14" s="123" t="s">
+      <c r="F14" s="122" t="s">
         <v>563</v>
       </c>
-      <c r="G14" s="123" t="n">
+      <c r="G14" s="122" t="n">
         <v>0.00058</v>
       </c>
-      <c r="H14" s="123" t="n">
+      <c r="H14" s="122" t="n">
         <v>0.625</v>
       </c>
-      <c r="I14" s="123" t="s">
+      <c r="I14" s="122" t="s">
         <v>564</v>
       </c>
       <c r="J14" s="0" t="s">
@@ -5840,25 +5862,25 @@
       <c r="A15" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="C15" s="122" t="s">
+      <c r="C15" s="121" t="s">
         <v>566</v>
       </c>
-      <c r="D15" s="123" t="s">
+      <c r="D15" s="122" t="s">
         <v>562</v>
       </c>
-      <c r="E15" s="122" t="n">
+      <c r="E15" s="121" t="n">
         <v>0.5</v>
       </c>
-      <c r="F15" s="122" t="n">
+      <c r="F15" s="121" t="n">
         <v>5</v>
       </c>
-      <c r="G15" s="122" t="n">
+      <c r="G15" s="121" t="n">
         <v>0.1</v>
       </c>
-      <c r="H15" s="122" t="n">
+      <c r="H15" s="121" t="n">
         <v>4</v>
       </c>
-      <c r="I15" s="122" t="s">
+      <c r="I15" s="121" t="s">
         <v>567</v>
       </c>
       <c r="J15" s="0" t="s">
@@ -5869,28 +5891,28 @@
       <c r="A16" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="C16" s="123" t="s">
+      <c r="C16" s="122" t="s">
         <v>569</v>
       </c>
-      <c r="D16" s="123" t="s">
+      <c r="D16" s="122" t="s">
         <v>570</v>
       </c>
-      <c r="E16" s="123" t="n">
+      <c r="E16" s="122" t="n">
         <v>0.137</v>
       </c>
-      <c r="F16" s="123" t="s">
+      <c r="F16" s="122" t="s">
         <v>571</v>
       </c>
-      <c r="G16" s="123" t="n">
+      <c r="G16" s="122" t="n">
         <v>0.02</v>
       </c>
-      <c r="H16" s="123" t="n">
-        <v>0</v>
-      </c>
-      <c r="I16" s="123" t="s">
+      <c r="H16" s="122" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" s="122" t="s">
         <v>572</v>
       </c>
-      <c r="J16" s="124" t="s">
+      <c r="J16" s="123" t="s">
         <v>573</v>
       </c>
     </row>
@@ -5898,28 +5920,28 @@
       <c r="A17" s="0" t="n">
         <v>12</v>
       </c>
-      <c r="C17" s="123" t="s">
+      <c r="C17" s="122" t="s">
         <v>574</v>
       </c>
-      <c r="D17" s="123" t="s">
+      <c r="D17" s="122" t="s">
         <v>575</v>
       </c>
-      <c r="E17" s="123" t="n">
+      <c r="E17" s="122" t="n">
         <v>0.06</v>
       </c>
-      <c r="F17" s="123" t="n">
+      <c r="F17" s="122" t="n">
         <v>0.23</v>
       </c>
-      <c r="G17" s="123" t="n">
+      <c r="G17" s="122" t="n">
         <v>0.0017</v>
       </c>
-      <c r="H17" s="123" t="n">
+      <c r="H17" s="122" t="n">
         <v>0.15</v>
       </c>
-      <c r="I17" s="123" t="s">
+      <c r="I17" s="122" t="s">
         <v>576</v>
       </c>
-      <c r="J17" s="124" t="s">
+      <c r="J17" s="123" t="s">
         <v>577</v>
       </c>
     </row>
@@ -5927,28 +5949,28 @@
       <c r="A18" s="0" t="n">
         <v>13</v>
       </c>
-      <c r="C18" s="123" t="s">
+      <c r="C18" s="122" t="s">
         <v>578</v>
       </c>
-      <c r="D18" s="123" t="s">
+      <c r="D18" s="122" t="s">
         <v>575</v>
       </c>
-      <c r="E18" s="123" t="n">
+      <c r="E18" s="122" t="n">
         <v>0.09</v>
       </c>
-      <c r="F18" s="123" t="n">
+      <c r="F18" s="122" t="n">
         <v>2.3</v>
       </c>
-      <c r="G18" s="123" t="n">
+      <c r="G18" s="122" t="n">
         <v>0.0036</v>
       </c>
-      <c r="H18" s="123" t="n">
+      <c r="H18" s="122" t="n">
         <v>0.19</v>
       </c>
-      <c r="I18" s="123" t="s">
+      <c r="I18" s="122" t="s">
         <v>579</v>
       </c>
-      <c r="J18" s="124" t="s">
+      <c r="J18" s="123" t="s">
         <v>577</v>
       </c>
     </row>
@@ -5956,28 +5978,28 @@
       <c r="A19" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="C19" s="123" t="s">
+      <c r="C19" s="122" t="s">
         <v>580</v>
       </c>
-      <c r="D19" s="123" t="s">
+      <c r="D19" s="122" t="s">
         <v>575</v>
       </c>
-      <c r="E19" s="123" t="n">
+      <c r="E19" s="122" t="n">
         <v>0.15</v>
       </c>
-      <c r="F19" s="123" t="n">
+      <c r="F19" s="122" t="n">
         <v>1</v>
       </c>
-      <c r="G19" s="123" t="n">
+      <c r="G19" s="122" t="n">
         <v>0.01</v>
       </c>
-      <c r="H19" s="123" t="n">
+      <c r="H19" s="122" t="n">
         <v>0.19</v>
       </c>
-      <c r="I19" s="123" t="s">
+      <c r="I19" s="122" t="s">
         <v>581</v>
       </c>
-      <c r="J19" s="124" t="s">
+      <c r="J19" s="123" t="s">
         <v>577</v>
       </c>
     </row>
@@ -5985,31 +6007,31 @@
       <c r="A20" s="0" t="n">
         <v>15</v>
       </c>
-      <c r="B20" s="125" t="s">
+      <c r="B20" s="124" t="s">
         <v>582</v>
       </c>
-      <c r="C20" s="126" t="s">
+      <c r="C20" s="125" t="s">
         <v>583</v>
       </c>
-      <c r="D20" s="123" t="s">
+      <c r="D20" s="122" t="s">
         <v>584</v>
       </c>
-      <c r="E20" s="123" t="n">
+      <c r="E20" s="122" t="n">
         <v>0.694</v>
       </c>
-      <c r="F20" s="123" t="n">
+      <c r="F20" s="122" t="n">
         <v>0.635</v>
       </c>
-      <c r="G20" s="123" t="n">
+      <c r="G20" s="122" t="n">
         <v>0.0093</v>
       </c>
-      <c r="H20" s="123" t="n">
+      <c r="H20" s="122" t="n">
         <v>3.17</v>
       </c>
-      <c r="I20" s="123" t="s">
+      <c r="I20" s="122" t="s">
         <v>585</v>
       </c>
-      <c r="J20" s="124" t="s">
+      <c r="J20" s="123" t="s">
         <v>586</v>
       </c>
     </row>
@@ -6017,25 +6039,25 @@
       <c r="A21" s="0" t="n">
         <v>16</v>
       </c>
-      <c r="C21" s="123" t="s">
+      <c r="C21" s="122" t="s">
         <v>587</v>
       </c>
-      <c r="D21" s="123" t="s">
+      <c r="D21" s="122" t="s">
         <v>588</v>
       </c>
-      <c r="E21" s="123" t="n">
+      <c r="E21" s="122" t="n">
         <v>0.02</v>
       </c>
-      <c r="F21" s="123" t="n">
+      <c r="F21" s="122" t="n">
         <v>0.1</v>
       </c>
-      <c r="G21" s="123" t="n">
+      <c r="G21" s="122" t="n">
         <v>0.002</v>
       </c>
-      <c r="H21" s="123" t="n">
+      <c r="H21" s="122" t="n">
         <v>0.15</v>
       </c>
-      <c r="I21" s="123" t="s">
+      <c r="I21" s="122" t="s">
         <v>589</v>
       </c>
       <c r="J21" s="117" t="s">
@@ -6047,7 +6069,7 @@
       <c r="L21" s="0" t="s">
         <v>592</v>
       </c>
-      <c r="M21" s="127" t="s">
+      <c r="M21" s="126" t="s">
         <v>593</v>
       </c>
     </row>
@@ -6055,34 +6077,34 @@
       <c r="A22" s="0" t="n">
         <v>17</v>
       </c>
-      <c r="C22" s="123" t="s">
+      <c r="C22" s="122" t="s">
         <v>594</v>
       </c>
-      <c r="D22" s="123" t="s">
+      <c r="D22" s="122" t="s">
         <v>595</v>
       </c>
-      <c r="E22" s="123" t="n">
+      <c r="E22" s="122" t="n">
         <v>0.18</v>
       </c>
-      <c r="F22" s="123" t="n">
+      <c r="F22" s="122" t="n">
         <v>1.5</v>
       </c>
-      <c r="G22" s="123" t="n">
+      <c r="G22" s="122" t="n">
         <v>0.019</v>
       </c>
-      <c r="H22" s="123" t="n">
+      <c r="H22" s="122" t="n">
         <v>0.5</v>
       </c>
-      <c r="I22" s="123" t="s">
+      <c r="I22" s="122" t="s">
         <v>596</v>
       </c>
-      <c r="J22" s="124" t="s">
+      <c r="J22" s="123" t="s">
         <v>597</v>
       </c>
       <c r="K22" s="30" t="s">
         <v>598</v>
       </c>
-      <c r="M22" s="127" t="s">
+      <c r="M22" s="126" t="s">
         <v>593</v>
       </c>
     </row>
@@ -6090,32 +6112,32 @@
       <c r="A23" s="0" t="n">
         <v>18</v>
       </c>
-      <c r="C23" s="123" t="s">
+      <c r="C23" s="122" t="s">
         <v>599</v>
       </c>
-      <c r="D23" s="123" t="s">
+      <c r="D23" s="122" t="s">
         <v>600</v>
       </c>
-      <c r="E23" s="123"/>
-      <c r="F23" s="123" t="n">
+      <c r="E23" s="122"/>
+      <c r="F23" s="122" t="n">
         <v>0.5</v>
       </c>
-      <c r="G23" s="123" t="n">
+      <c r="G23" s="122" t="n">
         <v>0.004</v>
       </c>
-      <c r="H23" s="123" t="n">
+      <c r="H23" s="122" t="n">
         <v>0.6</v>
       </c>
-      <c r="I23" s="123" t="s">
+      <c r="I23" s="122" t="s">
         <v>601</v>
       </c>
-      <c r="J23" s="124" t="s">
+      <c r="J23" s="123" t="s">
         <v>602</v>
       </c>
       <c r="K23" s="30" t="s">
         <v>603</v>
       </c>
-      <c r="M23" s="127" t="s">
+      <c r="M23" s="126" t="s">
         <v>593</v>
       </c>
     </row>
@@ -6123,32 +6145,32 @@
       <c r="A24" s="0" t="n">
         <v>19</v>
       </c>
-      <c r="C24" s="123" t="s">
+      <c r="C24" s="122" t="s">
         <v>604</v>
       </c>
-      <c r="D24" s="123" t="s">
+      <c r="D24" s="122" t="s">
         <v>605</v>
       </c>
-      <c r="E24" s="123" t="n">
+      <c r="E24" s="122" t="n">
         <v>0.055</v>
       </c>
-      <c r="F24" s="123" t="n">
+      <c r="F24" s="122" t="n">
         <v>3</v>
       </c>
-      <c r="G24" s="123" t="n">
+      <c r="G24" s="122" t="n">
         <v>0.015</v>
       </c>
-      <c r="H24" s="123"/>
-      <c r="I24" s="123" t="s">
+      <c r="H24" s="122"/>
+      <c r="I24" s="122" t="s">
         <v>606</v>
       </c>
-      <c r="J24" s="124" t="s">
+      <c r="J24" s="123" t="s">
         <v>607</v>
       </c>
       <c r="K24" s="30" t="s">
         <v>525</v>
       </c>
-      <c r="M24" s="128" t="s">
+      <c r="M24" s="127" t="s">
         <v>608</v>
       </c>
     </row>
@@ -6156,28 +6178,28 @@
       <c r="A25" s="0" t="n">
         <v>20</v>
       </c>
-      <c r="C25" s="123" t="s">
+      <c r="C25" s="122" t="s">
         <v>609</v>
       </c>
-      <c r="D25" s="123" t="s">
+      <c r="D25" s="122" t="s">
         <v>610</v>
       </c>
-      <c r="E25" s="123" t="n">
+      <c r="E25" s="122" t="n">
         <v>0.26</v>
       </c>
-      <c r="F25" s="123" t="n">
+      <c r="F25" s="122" t="n">
         <v>4</v>
       </c>
-      <c r="G25" s="123" t="n">
+      <c r="G25" s="122" t="n">
         <v>0.04</v>
       </c>
-      <c r="H25" s="123" t="n">
+      <c r="H25" s="122" t="n">
         <v>0.5</v>
       </c>
-      <c r="I25" s="123" t="s">
+      <c r="I25" s="122" t="s">
         <v>611</v>
       </c>
-      <c r="J25" s="124"/>
+      <c r="J25" s="123"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6204,14 +6226,14 @@
   </sheetPr>
   <dimension ref="B1:H40"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K24" activeCellId="0" sqref="K24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.3886639676113"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="7" min="4" style="0" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.3562753036437"/>
@@ -6219,20 +6241,20 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="129"/>
-      <c r="C1" s="129"/>
-      <c r="D1" s="129"/>
-      <c r="E1" s="129"/>
-      <c r="F1" s="129"/>
-      <c r="G1" s="129"/>
+      <c r="B1" s="128"/>
+      <c r="C1" s="128"/>
+      <c r="D1" s="128"/>
+      <c r="E1" s="128"/>
+      <c r="F1" s="128"/>
+      <c r="G1" s="128"/>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="130"/>
-      <c r="C2" s="130"/>
-      <c r="D2" s="130"/>
-      <c r="E2" s="130"/>
-      <c r="F2" s="130"/>
-      <c r="G2" s="130"/>
+      <c r="B2" s="129"/>
+      <c r="C2" s="129"/>
+      <c r="D2" s="129"/>
+      <c r="E2" s="129"/>
+      <c r="F2" s="129"/>
+      <c r="G2" s="129"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="117"/>
@@ -6267,164 +6289,164 @@
       <c r="G6" s="117"/>
     </row>
     <row r="10" customFormat="false" ht="14.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B10" s="121" t="s">
+      <c r="B10" s="130" t="s">
         <v>612</v>
       </c>
-      <c r="C10" s="121"/>
-      <c r="D10" s="121"/>
-      <c r="E10" s="121"/>
-      <c r="F10" s="121"/>
-      <c r="G10" s="121"/>
-      <c r="H10" s="123"/>
+      <c r="C10" s="130"/>
+      <c r="D10" s="130"/>
+      <c r="E10" s="130"/>
+      <c r="F10" s="130"/>
+      <c r="G10" s="130"/>
+      <c r="H10" s="131"/>
     </row>
     <row r="11" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="116" t="s">
+      <c r="B11" s="132" t="s">
         <v>134</v>
       </c>
-      <c r="C11" s="116" t="s">
+      <c r="C11" s="132" t="s">
         <v>135</v>
       </c>
-      <c r="D11" s="116" t="s">
+      <c r="D11" s="132" t="s">
         <v>613</v>
       </c>
-      <c r="E11" s="116" t="s">
+      <c r="E11" s="132" t="s">
         <v>138</v>
       </c>
-      <c r="F11" s="116" t="s">
+      <c r="F11" s="132" t="s">
         <v>614</v>
       </c>
-      <c r="G11" s="116" t="s">
+      <c r="G11" s="132" t="s">
         <v>615</v>
       </c>
-      <c r="H11" s="116" t="s">
+      <c r="H11" s="132" t="s">
         <v>529</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="122" t="s">
+    <row r="12" customFormat="false" ht="14.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="133" t="s">
         <v>616</v>
       </c>
-      <c r="C12" s="122" t="s">
+      <c r="C12" s="133" t="s">
         <v>617</v>
       </c>
-      <c r="D12" s="122" t="s">
+      <c r="D12" s="133" t="s">
         <v>618</v>
       </c>
-      <c r="E12" s="122" t="s">
+      <c r="E12" s="133" t="s">
         <v>619</v>
       </c>
-      <c r="F12" s="122" t="n">
+      <c r="F12" s="133" t="n">
         <v>1160</v>
       </c>
-      <c r="G12" s="122" t="s">
+      <c r="G12" s="133" t="s">
         <v>620</v>
       </c>
-      <c r="H12" s="123" t="s">
+      <c r="H12" s="131" t="s">
         <v>621</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="122" t="s">
+    <row r="13" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="133" t="s">
         <v>622</v>
       </c>
-      <c r="C13" s="122" t="s">
+      <c r="C13" s="133" t="s">
         <v>623</v>
       </c>
-      <c r="D13" s="122" t="s">
+      <c r="D13" s="133" t="s">
         <v>624</v>
       </c>
-      <c r="E13" s="122" t="n">
+      <c r="E13" s="133" t="n">
         <v>2</v>
       </c>
-      <c r="F13" s="122" t="n">
+      <c r="F13" s="133" t="n">
         <v>655</v>
       </c>
-      <c r="G13" s="122" t="n">
+      <c r="G13" s="133" t="n">
         <v>280</v>
       </c>
-      <c r="H13" s="131"/>
-    </row>
-    <row r="14" customFormat="false" ht="41.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="122" t="s">
+      <c r="H13" s="134"/>
+    </row>
+    <row r="14" customFormat="false" ht="41.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="133" t="s">
         <v>625</v>
       </c>
-      <c r="C14" s="122" t="s">
+      <c r="C14" s="133" t="s">
         <v>626</v>
       </c>
-      <c r="D14" s="122" t="s">
+      <c r="D14" s="133" t="s">
         <v>627</v>
       </c>
-      <c r="E14" s="122" t="s">
+      <c r="E14" s="133" t="s">
         <v>619</v>
       </c>
-      <c r="F14" s="122" t="n">
+      <c r="F14" s="133" t="n">
         <v>536</v>
       </c>
-      <c r="G14" s="122"/>
-      <c r="H14" s="123"/>
-    </row>
-    <row r="15" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="122" t="s">
+      <c r="G14" s="133"/>
+      <c r="H14" s="131"/>
+    </row>
+    <row r="15" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="133" t="s">
         <v>628</v>
       </c>
-      <c r="C15" s="122" t="s">
+      <c r="C15" s="133" t="s">
         <v>629</v>
       </c>
-      <c r="D15" s="122" t="s">
+      <c r="D15" s="133" t="s">
         <v>630</v>
       </c>
-      <c r="E15" s="122" t="n">
+      <c r="E15" s="133" t="n">
         <v>100</v>
       </c>
-      <c r="F15" s="122" t="s">
+      <c r="F15" s="133" t="s">
         <v>631</v>
       </c>
-      <c r="G15" s="122"/>
-      <c r="H15" s="123"/>
+      <c r="G15" s="133"/>
+      <c r="H15" s="131"/>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="123" t="s">
+      <c r="B16" s="131" t="s">
         <v>632</v>
       </c>
-      <c r="C16" s="123" t="s">
+      <c r="C16" s="131" t="s">
         <v>633</v>
       </c>
-      <c r="D16" s="123" t="s">
+      <c r="D16" s="131" t="s">
         <v>634</v>
       </c>
-      <c r="E16" s="123" t="n">
+      <c r="E16" s="131" t="n">
         <v>2</v>
       </c>
-      <c r="F16" s="123" t="n">
+      <c r="F16" s="131" t="n">
         <v>110</v>
       </c>
-      <c r="G16" s="123" t="n">
+      <c r="G16" s="131" t="n">
         <v>350</v>
       </c>
-      <c r="H16" s="123" t="s">
+      <c r="H16" s="131" t="s">
         <v>585</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="123" t="s">
+      <c r="B17" s="131" t="s">
         <v>635</v>
       </c>
-      <c r="C17" s="123" t="s">
+      <c r="C17" s="131" t="s">
         <v>633</v>
       </c>
-      <c r="D17" s="123" t="s">
+      <c r="D17" s="131" t="s">
         <v>636</v>
       </c>
-      <c r="E17" s="123" t="n">
+      <c r="E17" s="131" t="n">
         <v>2</v>
       </c>
-      <c r="F17" s="123" t="n">
+      <c r="F17" s="131" t="n">
         <v>110</v>
       </c>
-      <c r="G17" s="123" t="n">
+      <c r="G17" s="131" t="n">
         <v>900</v>
       </c>
-      <c r="H17" s="123" t="s">
+      <c r="H17" s="131" t="s">
         <v>637</v>
       </c>
     </row>
@@ -6458,7 +6480,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9595141700405"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.0688259109312"/>
     <col collapsed="false" hidden="false" max="5" min="3" style="0" width="8.57085020242915"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="4.92712550607287"/>
     <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="8.57085020242915"/>
@@ -6657,10 +6679,10 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="24.7449392712551"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.3117408906883"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="36.6356275303644"/>
     <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -6967,20 +6989,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.5303643724696"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="24.7449392712551"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.9271255060729"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.3522267206478"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.1740890688259"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.6396761133603"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="20.4615384615385"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="19.3886639676113"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="18.7449392712551"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.5668016194332"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.4251012145749"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.4939271255061"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="17.6761133603239"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="19.6032388663968"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="0" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.1376518218623"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="20.246963562753"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="0" width="10.6032388663968"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="12.9595141700405"/>
     <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>
@@ -7853,27 +7875,27 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.7085020242915"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.8137651821862"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="10.497975708502"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.8542510121457"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="18.9595141700405"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="6" min="6" style="0" width="4.92712550607287"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="0" width="4.92712550607287"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="0" width="4.92712550607287"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="18" min="18" style="0" width="4.92712550607287"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.5303643724696"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="0" width="15.6396761133603"/>
     <col collapsed="false" hidden="false" max="20" min="20" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.3198380566802"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="0" width="15.4251012145749"/>
     <col collapsed="false" hidden="false" max="22" min="22" style="0" width="4.92712550607287"/>
     <col collapsed="false" hidden="false" max="1025" min="23" style="0" width="8.57085020242915"/>
   </cols>
@@ -10237,7 +10259,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.57085020242915"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.9595141700405"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="4" style="0" width="8.57085020242915"/>
   </cols>
@@ -10294,7 +10316,7 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="6" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.3198380566802"/>
     <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData>
@@ -10670,7 +10692,7 @@
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="6" min="1" style="0" width="9.10526315789474"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="12.3198380566802"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="0" width="11.4615384615385"/>
     <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="9.10526315789474"/>
   </cols>

</xml_diff>